<commit_message>
vault backup: 2026-01-20 17:32:15
</commit_message>
<xml_diff>
--- a/de/design_spec/ref/linting table.xlsx
+++ b/de/design_spec/ref/linting table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\project\AI\1_HW_AnDLA\0_Meeting\00_others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\obs\de\design_spec\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFA823A-7C94-48E5-837C-09B38E597DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F0FF4F-7CEB-429C-B0FE-1BCA59F4CAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="29676" windowHeight="17496" tabRatio="878" xr2:uid="{56A7BD0B-C13C-4886-8618-7B2B37719770}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="878" xr2:uid="{56A7BD0B-C13C-4886-8618-7B2B37719770}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="38" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="180">
   <si>
     <t>explaint</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1007,18 +1007,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1032,14 +1032,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1047,7 +1047,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1055,7 +1055,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1084,7 +1084,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1216,12 +1216,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1" xr:uid="{59A10125-9653-4B3E-B7F4-1A01EC37A389}"/>
+    <cellStyle name="中等" xfId="4" builtinId="28"/>
+    <cellStyle name="壞" xfId="3" builtinId="27"/>
+    <cellStyle name="好" xfId="2" builtinId="26"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -1786,7 +1786,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -2084,28 +2084,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99935B7A-BA07-42AA-B138-6FEA23F2A251}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="29" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="111.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="66.296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="31.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69921875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.69921875" style="5"/>
-    <col min="9" max="9" width="24.59765625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="26.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="124.19921875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.69921875" style="5"/>
+    <col min="1" max="1" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="31.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="5"/>
+    <col min="9" max="9" width="24.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="26.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="124.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>80</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>111</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>112</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>113</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>102</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>114</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.2">
+    <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>115</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:7" s="11" customFormat="1" ht="16.2">
+    <row r="8" spans="1:7" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -2257,7 +2257,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="16.2">
+    <row r="9" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>77</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>78</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.2">
+    <row r="11" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>116</v>
       </c>
@@ -2309,7 +2309,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>74</v>
       </c>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="16.2">
+    <row r="13" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>117</v>
       </c>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="16.2">
+    <row r="14" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>87</v>
       </c>
@@ -2360,8 +2360,11 @@
       <c r="F14" s="10" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.2">
+      <c r="G14" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>94</v>
       </c>
@@ -2378,8 +2381,11 @@
       <c r="F15" s="10" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="G15" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>83</v>
       </c>
@@ -2395,7 +2401,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>177</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>31</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" customHeight="1">
+    <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>34</v>
       </c>
@@ -2443,7 +2449,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>37</v>
       </c>
@@ -2457,7 +2463,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="16.2">
+    <row r="21" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16.2">
+    <row r="22" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>178</v>
       </c>
@@ -2500,7 +2506,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.2">
+    <row r="23" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>118</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.2">
+    <row r="24" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>119</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>120</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>121</v>
       </c>
@@ -2586,7 +2592,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>122</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>98</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>123</v>
       </c>
@@ -2644,7 +2650,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>29</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>124</v>
       </c>
@@ -2690,7 +2696,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>103</v>
       </c>
@@ -2704,7 +2710,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>125</v>
       </c>
@@ -2718,7 +2724,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>33</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16.2">
+    <row r="35" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>126</v>
       </c>
@@ -2755,7 +2761,7 @@
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="1:7" ht="16.2">
+    <row r="36" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>90</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.2">
+    <row r="37" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>127</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>172</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="31.2">
+    <row r="41" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>173</v>
       </c>
@@ -2826,18 +2832,18 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="133.296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.69921875" style="1"/>
+    <col min="1" max="1" width="30.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="133.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1"/>
     <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.69921875" style="1"/>
+    <col min="6" max="6" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>79</v>
       </c>
@@ -2848,7 +2854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2859,7 +2865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2969,7 +2975,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -3002,7 +3008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
@@ -3013,7 +3019,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
@@ -3079,7 +3085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>55</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -3134,7 +3140,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="46.8">
+    <row r="28" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
@@ -3145,7 +3151,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3173,14 +3179,14 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="133.296875" customWidth="1"/>
-    <col min="3" max="3" width="34.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="133.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>80</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3202,7 +3208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3213,7 +3219,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3224,7 +3230,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -3235,7 +3241,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>74</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3257,7 +3263,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -3268,7 +3274,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>78</v>
       </c>
@@ -3279,7 +3285,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
@@ -3301,7 +3307,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>84</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -3323,7 +3329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -3334,7 +3340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -3367,7 +3373,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5" customHeight="1">
+    <row r="18" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>99</v>
       </c>
@@ -3378,7 +3384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -3389,7 +3395,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3400,7 +3406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.55" customHeight="1">
+    <row r="22" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -3422,7 +3428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17.55" customHeight="1">
+    <row r="23" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>91</v>
       </c>
@@ -3433,7 +3439,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>65</v>
       </c>
@@ -3461,14 +3467,14 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="120.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>80</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>74</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>78</v>
       </c>
@@ -3567,7 +3573,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
@@ -3589,7 +3595,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>84</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -3622,7 +3628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3644,7 +3650,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>99</v>
       </c>
@@ -3666,7 +3672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -3677,7 +3683,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3688,7 +3694,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>91</v>
       </c>
@@ -3721,7 +3727,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>65</v>
       </c>
@@ -3732,27 +3738,27 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3774,14 +3780,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>80</v>
       </c>
@@ -3792,7 +3798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3814,7 +3820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3847,7 +3853,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>78</v>
       </c>
@@ -3858,7 +3864,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>87</v>
       </c>
@@ -3869,7 +3875,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
@@ -3880,7 +3886,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3902,7 +3908,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -3913,7 +3919,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -3935,7 +3941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>99</v>
       </c>
@@ -3946,7 +3952,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>55</v>
       </c>
@@ -3957,7 +3963,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -3968,7 +3974,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
@@ -3979,7 +3985,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>104</v>
       </c>
@@ -3990,7 +3996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -4001,7 +4007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>91</v>
       </c>
@@ -4012,7 +4018,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
@@ -4023,27 +4029,27 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-20 17:42:23
</commit_message>
<xml_diff>
--- a/de/design_spec/ref/linting table.xlsx
+++ b/de/design_spec/ref/linting table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\obs\de\design_spec\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F0FF4F-7CEB-429C-B0FE-1BCA59F4CAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A9EB45-4989-43E3-980A-B5DE53F120C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="878" xr2:uid="{56A7BD0B-C13C-4886-8618-7B2B37719770}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="181">
   <si>
     <t>explaint</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -964,9 +964,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MarsV2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Port connections in instantiations must be made by named association rather than positional association. </t>
   </si>
   <si>
@@ -1002,12 +999,20 @@
       <t>(kv_clkdiv.v, sample_kv_clk_gen.v)</t>
     </r>
   </si>
+  <si>
+    <t>only for genclk module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnDLA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1096,8 +1101,16 @@
       <family val="1"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1125,8 +1138,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1149,8 +1168,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1167,8 +1306,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1190,9 +1332,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1208,14 +1347,51 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="60% - 輔色1" xfId="6" builtinId="32"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1" xr:uid="{59A10125-9653-4B3E-B7F4-1A01EC37A389}"/>
     <cellStyle name="中等" xfId="4" builtinId="28"/>
@@ -2084,11 +2260,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99935B7A-BA07-42AA-B138-6FEA23F2A251}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="29" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2097,7 +2273,7 @@
     <col min="2" max="2" width="111.44140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="31.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="24" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" style="5"/>
     <col min="9" max="9" width="24.5546875" style="5" customWidth="1"/>
     <col min="10" max="10" width="26.77734375" style="5" bestFit="1" customWidth="1"/>
@@ -2105,705 +2281,726 @@
     <col min="12" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="24" t="s">
         <v>168</v>
       </c>
+      <c r="G37" s="25"/>
     </row>
     <row r="39" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2812,7 +3009,7 @@
         <v>173</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2026-01-20 18:02:40
</commit_message>
<xml_diff>
--- a/de/design_spec/ref/linting table.xlsx
+++ b/de/design_spec/ref/linting table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\obs\de\design_spec\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A9EB45-4989-43E3-980A-B5DE53F120C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA938FFB-8A67-43A9-ACF1-3C05CD10DF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="878" xr2:uid="{56A7BD0B-C13C-4886-8618-7B2B37719770}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="181">
   <si>
     <t>explaint</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2264,7 +2264,7 @@
       <pane xSplit="2" ySplit="29" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2634,7 +2634,9 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">

</xml_diff>

<commit_message>
vault backup: 2026-01-20 19:29:54
</commit_message>
<xml_diff>
--- a/de/design_spec/ref/linting table.xlsx
+++ b/de/design_spec/ref/linting table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\obs\de\design_spec\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA938FFB-8A67-43A9-ACF1-3C05CD10DF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992BA2C-A9D6-4CB4-A62B-35B71AA1B873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="878" xr2:uid="{56A7BD0B-C13C-4886-8618-7B2B37719770}"/>
   </bookViews>
@@ -2264,7 +2264,7 @@
       <pane xSplit="2" ySplit="29" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>